<commit_message>
Updated task list to make me do work.
</commit_message>
<xml_diff>
--- a/Project Management/Costing.xlsx
+++ b/Project Management/Costing.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Costing" sheetId="1" r:id="rId1"/>
+    <sheet name="To Do List" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>BFNG</t>
   </si>
@@ -67,6 +67,45 @@
   </si>
   <si>
     <t>Arduino Yun</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>CAD of tripod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop servo system </t>
+  </si>
+  <si>
+    <t>Develop trigger system</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Wait for beginner package</t>
+  </si>
+  <si>
+    <t>Do tutorials</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Merge servo and trigger onto expansion board</t>
+  </si>
+  <si>
+    <t>Research 7 segment displays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count functions for bullets fired. </t>
   </si>
 </sst>
 </file>
@@ -102,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +163,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,15 +224,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -199,30 +238,38 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -534,7 +581,7 @@
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -543,182 +590,182 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="9">
         <v>50</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="10">
         <v>20</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="9">
         <v>139</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="11">
         <v>84.27</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="9">
         <f>SUM(C5:C16)</f>
         <v>189</v>
       </c>
@@ -728,10 +775,10 @@
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="6:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="9">
         <f>SUM(D5:D15)</f>
         <v>104.27</v>
       </c>
@@ -741,15 +788,15 @@
       <c r="I17" s="12"/>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="8">
         <f>SUM(E5:E15)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -766,12 +813,244 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>42027</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>